<commit_message>
fix the reports functionality and generated dtr mail
</commit_message>
<xml_diff>
--- a/public/templates/iDtr_result - John Vincent Ramada.xlsx
+++ b/public/templates/iDtr_result - John Vincent Ramada.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <r>
       <t xml:space="preserve">Civil Service Form No. 48                                                                 </t>
@@ -52,13 +52,13 @@
     <t>---------------</t>
   </si>
   <si>
-    <t>John Vincent Ramiso Ramada</t>
+    <t>John Vincent ramiso ramada</t>
   </si>
   <si>
     <t>(Name)</t>
   </si>
   <si>
-    <t>For the month of February - March</t>
+    <t>For the month of March - March</t>
   </si>
   <si>
     <r>
@@ -167,13 +167,7 @@
     <t>Minutes</t>
   </si>
   <si>
-    <t>10:08</t>
-  </si>
-  <si>
-    <t>12:21</t>
-  </si>
-  <si>
-    <t>2:21</t>
+    <t>11:11</t>
   </si>
   <si>
     <t>(SEE INSTRUCTION ON BACK)</t>
@@ -1246,7 +1240,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="130" zoomScaleNormal="130" showGridLines="true" showRowColHeaders="1" topLeftCell="A3">
       <selection activeCell="B15" sqref="B15:H15"/>
@@ -1397,17 +1391,15 @@
         <v>16</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="7">
-        <v>2</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" customHeight="1" ht="15.75">
@@ -1565,9 +1557,7 @@
       <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B27" s="6">
-        <v>16</v>
-      </c>
+      <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
       <c r="E27" s="7"/>
@@ -1576,341 +1566,101 @@
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B28" s="6">
+      <c r="B28" s="11"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="1:8" customHeight="1" ht="16.5">
+      <c r="B29" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="9">
+        <f>SUM(G12:G28)</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="9">
+        <f>SUM(H12:H28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" customHeight="1" ht="24">
+      <c r="B30" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="26"/>
+    </row>
+    <row r="31" spans="1:8" customHeight="1" ht="15.75">
+      <c r="B31" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="29"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="B32" s="30"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="32"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="B33" s="33"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="35"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="B34" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="38"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="B35" s="62"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="64"/>
+    </row>
+    <row r="36" spans="1:8" customHeight="1" ht="15.75">
+      <c r="B36" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B29" s="6">
-        <v>18</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B30" s="6">
-        <v>19</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B31" s="6">
-        <v>20</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-    </row>
-    <row r="32" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B32" s="6">
-        <v>21</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-    </row>
-    <row r="33" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B33" s="6">
-        <v>22</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B34" s="6">
-        <v>23</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-    </row>
-    <row r="35" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B35" s="6">
-        <v>24</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-    </row>
-    <row r="36" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B36" s="6">
-        <v>25</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-    </row>
-    <row r="37" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B37" s="6">
-        <v>26</v>
-      </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-    </row>
-    <row r="38" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B38" s="6">
-        <v>27</v>
-      </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-    </row>
-    <row r="39" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B39" s="6">
-        <v>28</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-    </row>
-    <row r="40" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B40" s="6">
-        <v>29</v>
-      </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B41" s="6">
-        <v>30</v>
-      </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-    </row>
-    <row r="42" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B42" s="6">
-        <v>31</v>
-      </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-    </row>
-    <row r="43" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B43" s="6">
-        <v>32</v>
-      </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-    </row>
-    <row r="44" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B44" s="6">
-        <v>33</v>
-      </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-    </row>
-    <row r="45" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B45" s="6">
-        <v>34</v>
-      </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-    </row>
-    <row r="46" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B46" s="6">
-        <v>35</v>
-      </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B47" s="6">
-        <v>36</v>
-      </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-    </row>
-    <row r="48" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B48" s="6">
-        <v>37</v>
-      </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B49" s="6"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-    </row>
-    <row r="50" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B50" s="11"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-    </row>
-    <row r="51" spans="1:8" customHeight="1" ht="16.5">
-      <c r="B51" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" s="48"/>
-      <c r="D51" s="48"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="9">
-        <f>SUM(G12:G50)</f>
-        <v>2</v>
-      </c>
-      <c r="H51" s="9">
-        <f>SUM(H12:H50)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" customHeight="1" ht="24">
-      <c r="B52" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="26"/>
-    </row>
-    <row r="53" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B53" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="28"/>
-      <c r="H53" s="29"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="B54" s="30"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="32"/>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="B55" s="33"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="34"/>
-      <c r="H55" s="35"/>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="B56" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C56" s="37"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="38"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="B57" s="62"/>
-      <c r="C57" s="63"/>
-      <c r="D57" s="63"/>
-      <c r="E57" s="63"/>
-      <c r="F57" s="63"/>
-      <c r="G57" s="63"/>
-      <c r="H57" s="64"/>
-    </row>
-    <row r="58" spans="1:8" customHeight="1" ht="15.75">
-      <c r="B58" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="14"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="14"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -1918,22 +1668,22 @@
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B57:H57"/>
-    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B36:H36"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="B53:H53"/>
-    <mergeCell ref="B54:H54"/>
-    <mergeCell ref="B55:H55"/>
-    <mergeCell ref="B56:H56"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
     <mergeCell ref="B8:H8"/>
     <mergeCell ref="B9:H9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B29:F29"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>